<commit_message>
test case for bug 179 and 425
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/book/425-updateStyle.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/book/425-updateStyle.xlsx
@@ -26,11 +26,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -44,7 +43,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -52,18 +51,9 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill>
-        <fgColor rgb="FF996699"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF996699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF339900"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,14 +71,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -387,12 +374,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s" s="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>